<commit_message>
changed codice_eyetr_museo to match participant folder names in all_gaze
</commit_message>
<xml_diff>
--- a/data/demographic.xlsx
+++ b/data/demographic.xlsx
@@ -64,7 +64,7 @@
     <t>2021_2am</t>
   </si>
   <si>
-    <t>2021_2bm</t>
+    <t>2021_02bm</t>
   </si>
   <si>
     <t>Medicina</t>
@@ -82,7 +82,7 @@
     <t>2021_1am</t>
   </si>
   <si>
-    <t>2021_1bm</t>
+    <t>2021_01bm</t>
   </si>
   <si>
     <t>2021_3a</t>
@@ -103,7 +103,7 @@
     <t>2021_4am</t>
   </si>
   <si>
-    <t>2021_4bm</t>
+    <t>2021_04bm</t>
   </si>
   <si>
     <t>2021_4a</t>
@@ -115,7 +115,7 @@
     <t>2021_5am</t>
   </si>
   <si>
-    <t>2021_5bm</t>
+    <t>2021_05bmnew</t>
   </si>
   <si>
     <t>Maturità scientifica</t>
@@ -133,7 +133,7 @@
     <t>2021_3am</t>
   </si>
   <si>
-    <t>2021_3bm</t>
+    <t>2021_03bm</t>
   </si>
   <si>
     <t>2022_21av</t>
@@ -157,7 +157,7 @@
     <t>2021_1amf</t>
   </si>
   <si>
-    <t>2021_1bmf</t>
+    <t>2021_01bmf</t>
   </si>
   <si>
     <t>2022_5av</t>
@@ -169,7 +169,7 @@
     <t>2021_2amf</t>
   </si>
   <si>
-    <t>2021_2bmf</t>
+    <t>2021_02bmf</t>
   </si>
   <si>
     <t xml:space="preserve">Scienze Archeologiche </t>
@@ -250,7 +250,7 @@
     <t>2022_01am</t>
   </si>
   <si>
-    <t>2022_01bm</t>
+    <t>2022_01bmnew</t>
   </si>
   <si>
     <t xml:space="preserve">Igiene dentale </t>
@@ -610,7 +610,7 @@
     <t>2022_30am</t>
   </si>
   <si>
-    <t>2022_30bm</t>
+    <t>2022_30bm_</t>
   </si>
   <si>
     <t xml:space="preserve">economia </t>
@@ -694,7 +694,7 @@
     <t>2022_41am</t>
   </si>
   <si>
-    <t>2022_41bm</t>
+    <t>2022-41bm</t>
   </si>
   <si>
     <t xml:space="preserve">psicologia </t>
@@ -721,7 +721,7 @@
     <t>2022_38am</t>
   </si>
   <si>
-    <t>2022_38bm</t>
+    <t>2022_38bmnew</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,13 +739,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -803,7 +797,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1132,7 +1126,7 @@
     <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
synced codice_eyetr_museo with participant_folder
</commit_message>
<xml_diff>
--- a/data/demographic.xlsx
+++ b/data/demographic.xlsx
@@ -64,7 +64,7 @@
     <t>2021_2am</t>
   </si>
   <si>
-    <t>2021_02bm</t>
+    <t>2021_2bm</t>
   </si>
   <si>
     <t>Medicina</t>
@@ -82,7 +82,7 @@
     <t>2021_1am</t>
   </si>
   <si>
-    <t>2021_01bm</t>
+    <t>2021_1bm</t>
   </si>
   <si>
     <t>2021_3a</t>
@@ -103,7 +103,7 @@
     <t>2021_4am</t>
   </si>
   <si>
-    <t>2021_04bm</t>
+    <t>2021_4bm</t>
   </si>
   <si>
     <t>2021_4a</t>
@@ -133,7 +133,7 @@
     <t>2021_3am</t>
   </si>
   <si>
-    <t>2021_03bm</t>
+    <t>2021_3bm</t>
   </si>
   <si>
     <t>2022_21av</t>

</xml_diff>